<commit_message>
DESCW-1272: Project Recoveries - Admin Fees Tab 40
* Added Admin Fees Tab 40 report
* Added Admin Fees Tab 40 report to report selector
* Added Admin Fees Tab 40 report to report selector config
* updates model & helpers for Admin Fees Tab 40 report
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_40_rpt_PF_PortfolioAdminFees.xlsx
+++ b/backend/reports/xlsx/Tab_40_rpt_PF_PortfolioAdminFees.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C35190B-D3D7-3E42-9251-60B5732F9867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA57C2C-EE9A-534D-B0B8-7AFA5236F84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="-20320" windowWidth="25600" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>{#date=d.date}</t>
   </si>
@@ -50,15 +50,9 @@
     <t>{#rows=d.report[i+1]}</t>
   </si>
   <si>
-    <t>{#totals=d.report_totals[i]}</t>
-  </si>
-  <si>
     <t>Project Recoveries Admin Fees for {$fy} as of {$date}    (STOB - 8809 only)</t>
   </si>
   <si>
-    <t>Portfolio</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -105,13 +99,67 @@
   </si>
   <si>
     <t>{$p1}</t>
+  </si>
+  <si>
+    <t>{#subtotals=d.report[i].subtotals}</t>
+  </si>
+  <si>
+    <t>{#subtotals1=d.report[i].subtotals}</t>
+  </si>
+  <si>
+    <t>{$subtotals.q1}</t>
+  </si>
+  <si>
+    <t>{$subtotals.q2}</t>
+  </si>
+  <si>
+    <t>{$subtotals.q3}</t>
+  </si>
+  <si>
+    <t>{$subtotals.q4}</t>
+  </si>
+  <si>
+    <t>{$subtotals.total}</t>
+  </si>
+  <si>
+    <t>Grand Totals</t>
+  </si>
+  <si>
+    <t>{$grandTotals.total}</t>
+  </si>
+  <si>
+    <t>{$grandTotals.q4}</t>
+  </si>
+  <si>
+    <t>{$grandTotals.q3}</t>
+  </si>
+  <si>
+    <t>{$grandTotals.q2}</t>
+  </si>
+  <si>
+    <t>{$grandTotals.q1}</t>
+  </si>
+  <si>
+    <t>Portfolio Totals</t>
+  </si>
+  <si>
+    <t>{#grandTotals=d.grand_totals}</t>
+  </si>
+  <si>
+    <t>Project #</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>{$p.project_name}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -144,6 +192,26 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -177,7 +245,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -229,15 +297,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -248,11 +334,29 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -287,8 +391,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2411614</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>938414</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>680356</xdr:rowOff>
     </xdr:to>
@@ -632,137 +736,239 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="6" width="32.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" customWidth="1"/>
+    <col min="3" max="7" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="4"/>
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="24">
+      <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" ht="19">
+      <c r="A4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="19">
+      <c r="A5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" ht="19">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="24">
+      <c r="A7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" ht="19">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" ht="22" thickBot="1">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20" customHeight="1">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:7" ht="17">
+      <c r="A11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" ht="17">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" ht="17">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="17">
+      <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="21">
-      <c r="A3" s="9" t="s">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" ht="17">
+      <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" ht="17">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" ht="17">
+      <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" ht="17">
+      <c r="A18" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="21">
-      <c r="A6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-    </row>
-    <row r="9" spans="1:6" ht="17">
-      <c r="A9" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17">
-      <c r="A10" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="17">
-      <c r="A11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="17">
-      <c r="A12" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17">
-      <c r="A13" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="17">
-      <c r="A14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="17">
-      <c r="A15" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="17">
-      <c r="A16" s="5"/>
-    </row>
-    <row r="17" spans="1:1" ht="17">
-      <c r="A17" s="5" t="s">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" ht="17">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" ht="17">
+      <c r="A20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" ht="18" customHeight="1">
+      <c r="A21" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="17">
-      <c r="A18" s="5" t="s">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" ht="17">
+      <c r="A22" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="B22" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>

</xml_diff>